<commit_message>
71 körzet a pillanatnyilag elvárt minimum
</commit_message>
<xml_diff>
--- a/Összefogási opciók/2022-es választási összefogási opciók.xlsx
+++ b/Összefogási opciók/2022-es választási összefogási opciók.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">FIDESZ által éppen előírt körzeti jelöltek száma:</t>
   </si>
@@ -49,13 +49,7 @@
     <t xml:space="preserve">ÁTFEDÉSES KÖRZET</t>
   </si>
   <si>
-    <t xml:space="preserve">Előbbi 2 összege. El kell érje (most épp) az 50-et, hogy mindenki állíthasson listát:</t>
-  </si>
-  <si>
     <t xml:space="preserve">ÖSSZ. KÖRZET / PÁRT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A (pill.) 50-en felüli körzetek száma, amit a pártok egymásnak átadhatnak:</t>
   </si>
   <si>
     <t xml:space="preserve">ALKU TÁRGYA KÖRZET</t>
@@ -241,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -323,6 +317,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,14 +431,15 @@
   </sheetPr>
   <dimension ref="A1:L347"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A345" activeCellId="0" sqref="A345"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A325" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A174" activeCellId="0" sqref="A174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="7" style="0" width="11.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,8 +3217,9 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="15" t="s">
-        <v>9</v>
+      <c r="A117" s="15" t="str">
+        <f aca="false">"Előbbi 2 összege. El kell érje (most épp) a(z) "&amp;C1&amp;"-et, hogy mindenki állíthasson listát:"</f>
+        <v>Előbbi 2 összege. El kell érje (most épp) a(z) 71-et, hogy mindenki állíthasson listát:</v>
       </c>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>5</v>
@@ -4585,8 +4585,9 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="15" t="s">
-        <v>11</v>
+      <c r="A173" s="15" t="str">
+        <f aca="false">"A (pill.) "&amp;C1&amp;"-en felüli körzetek száma, amit a pártok egymásnak átadhatnak:"</f>
+        <v>A (pill.) 71-en felüli körzetek száma, amit a pártok egymásnak átadhatnak:</v>
       </c>
       <c r="B173" s="15"/>
       <c r="C173" s="15"/>
@@ -4596,7 +4597,7 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>5</v>
@@ -5953,7 +5954,7 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B229" s="15"/>
       <c r="C229" s="15"/>
@@ -5963,7 +5964,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B230" s="20"/>
       <c r="C230" s="20"/>
@@ -5973,7 +5974,7 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B231" s="15"/>
       <c r="C231" s="15"/>
@@ -5983,7 +5984,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B232" s="15"/>
       <c r="C232" s="15"/>
@@ -5993,7 +5994,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B233" s="3" t="s">
         <v>5</v>
@@ -6027,23 +6028,23 @@
       <c r="A235" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="B235" s="12" t="n">
+      <c r="B235" s="21" t="n">
         <f aca="false">AND((B176&lt;= B8),(B176 &gt;= 0),(B64&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C235" s="12" t="n">
+      <c r="C235" s="21" t="n">
         <f aca="false">AND((C176&lt;= C8),(C176 &gt;= 0),(C64&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D235" s="12" t="n">
+      <c r="D235" s="21" t="n">
         <f aca="false">AND((D176&lt;= D8),(D176 &gt;= 0),(D64&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E235" s="12" t="n">
+      <c r="E235" s="21" t="n">
         <f aca="false">AND((E176&lt;= E8),(E176 &gt;= 0),(E64&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F235" s="12" t="n">
+      <c r="F235" s="21" t="n">
         <f aca="false">AND((F176&lt;= F8),(F176 &gt;= 0),(F64&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6052,23 +6053,23 @@
       <c r="A236" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="B236" s="12" t="n">
+      <c r="B236" s="21" t="n">
         <f aca="false">AND((B177&lt;= B9),(B177 &gt;= 0),(B65&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C236" s="12" t="n">
+      <c r="C236" s="21" t="n">
         <f aca="false">AND((C177&lt;= C9),(C177 &gt;= 0),(C65&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D236" s="12" t="n">
+      <c r="D236" s="21" t="n">
         <f aca="false">AND((D177&lt;= D9),(D177 &gt;= 0),(D65&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E236" s="12" t="n">
+      <c r="E236" s="21" t="n">
         <f aca="false">AND((E177&lt;= E9),(E177 &gt;= 0),(E65&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F236" s="12" t="n">
+      <c r="F236" s="21" t="n">
         <f aca="false">AND((F177&lt;= F9),(F177 &gt;= 0),(F65&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6077,23 +6078,23 @@
       <c r="A237" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="B237" s="12" t="n">
+      <c r="B237" s="21" t="n">
         <f aca="false">AND((B178&lt;= B10),(B178 &gt;= 0),(B66&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C237" s="12" t="n">
+      <c r="C237" s="21" t="n">
         <f aca="false">AND((C178&lt;= C10),(C178 &gt;= 0),(C66&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D237" s="12" t="n">
+      <c r="D237" s="21" t="n">
         <f aca="false">AND((D178&lt;= D10),(D178 &gt;= 0),(D66&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E237" s="12" t="n">
+      <c r="E237" s="21" t="n">
         <f aca="false">AND((E178&lt;= E10),(E178 &gt;= 0),(E66&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F237" s="12" t="n">
+      <c r="F237" s="21" t="n">
         <f aca="false">AND((F178&lt;= F10),(F178 &gt;= 0),(F66&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6102,23 +6103,23 @@
       <c r="A238" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="B238" s="12" t="n">
+      <c r="B238" s="21" t="n">
         <f aca="false">AND((B179&lt;= B11),(B179 &gt;= 0),(B67&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C238" s="12" t="n">
+      <c r="C238" s="21" t="n">
         <f aca="false">AND((C179&lt;= C11),(C179 &gt;= 0),(C67&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D238" s="12" t="n">
+      <c r="D238" s="21" t="n">
         <f aca="false">AND((D179&lt;= D11),(D179 &gt;= 0),(D67&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E238" s="12" t="n">
+      <c r="E238" s="21" t="n">
         <f aca="false">AND((E179&lt;= E11),(E179 &gt;= 0),(E67&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="F238" s="12" t="n">
+      <c r="F238" s="21" t="n">
         <f aca="false">AND((F179&lt;= F11),(F179 &gt;= 0),(F67&gt;=0))</f>
         <v>1</v>
       </c>
@@ -6127,23 +6128,23 @@
       <c r="A239" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="B239" s="12" t="n">
+      <c r="B239" s="21" t="n">
         <f aca="false">AND((B180&lt;= B12),(B180 &gt;= 0),(B68&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C239" s="12" t="n">
+      <c r="C239" s="21" t="n">
         <f aca="false">AND((C180&lt;= C12),(C180 &gt;= 0),(C68&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D239" s="12" t="n">
+      <c r="D239" s="21" t="n">
         <f aca="false">AND((D180&lt;= D12),(D180 &gt;= 0),(D68&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E239" s="12" t="n">
+      <c r="E239" s="21" t="n">
         <f aca="false">AND((E180&lt;= E12),(E180 &gt;= 0),(E68&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="F239" s="12" t="n">
+      <c r="F239" s="21" t="n">
         <f aca="false">AND((F180&lt;= F12),(F180 &gt;= 0),(F68&gt;=0))</f>
         <v>1</v>
       </c>
@@ -6152,23 +6153,23 @@
       <c r="A240" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="B240" s="12" t="n">
+      <c r="B240" s="21" t="n">
         <f aca="false">AND((B181&lt;= B13),(B181 &gt;= 0),(B69&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C240" s="12" t="n">
+      <c r="C240" s="21" t="n">
         <f aca="false">AND((C181&lt;= C13),(C181 &gt;= 0),(C69&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D240" s="12" t="n">
+      <c r="D240" s="21" t="n">
         <f aca="false">AND((D181&lt;= D13),(D181 &gt;= 0),(D69&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E240" s="12" t="n">
+      <c r="E240" s="21" t="n">
         <f aca="false">AND((E181&lt;= E13),(E181 &gt;= 0),(E69&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="F240" s="12" t="n">
+      <c r="F240" s="21" t="n">
         <f aca="false">AND((F181&lt;= F13),(F181 &gt;= 0),(F69&gt;=0))</f>
         <v>1</v>
       </c>
@@ -6177,23 +6178,23 @@
       <c r="A241" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="B241" s="12" t="n">
+      <c r="B241" s="21" t="n">
         <f aca="false">AND((B182&lt;= B14),(B182 &gt;= 0),(B70&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C241" s="12" t="n">
+      <c r="C241" s="21" t="n">
         <f aca="false">AND((C182&lt;= C14),(C182 &gt;= 0),(C70&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D241" s="12" t="n">
+      <c r="D241" s="21" t="n">
         <f aca="false">AND((D182&lt;= D14),(D182 &gt;= 0),(D70&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E241" s="12" t="n">
+      <c r="E241" s="21" t="n">
         <f aca="false">AND((E182&lt;= E14),(E182 &gt;= 0),(E70&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="F241" s="12" t="n">
+      <c r="F241" s="21" t="n">
         <f aca="false">AND((F182&lt;= F14),(F182 &gt;= 0),(F70&gt;=0))</f>
         <v>1</v>
       </c>
@@ -6202,23 +6203,23 @@
       <c r="A242" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="B242" s="12" t="n">
+      <c r="B242" s="21" t="n">
         <f aca="false">AND((B183&lt;= B15),(B183 &gt;= 0),(B71&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C242" s="12" t="n">
+      <c r="C242" s="21" t="n">
         <f aca="false">AND((C183&lt;= C15),(C183 &gt;= 0),(C71&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D242" s="12" t="n">
+      <c r="D242" s="21" t="n">
         <f aca="false">AND((D183&lt;= D15),(D183 &gt;= 0),(D71&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E242" s="12" t="n">
+      <c r="E242" s="21" t="n">
         <f aca="false">AND((E183&lt;= E15),(E183 &gt;= 0),(E71&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="F242" s="12" t="n">
+      <c r="F242" s="21" t="n">
         <f aca="false">AND((F183&lt;= F15),(F183 &gt;= 0),(F71&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6227,23 +6228,23 @@
       <c r="A243" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="B243" s="12" t="n">
+      <c r="B243" s="21" t="n">
         <f aca="false">AND((B184&lt;= B16),(B184 &gt;= 0),(B72&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C243" s="12" t="n">
+      <c r="C243" s="21" t="n">
         <f aca="false">AND((C184&lt;= C16),(C184 &gt;= 0),(C72&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D243" s="12" t="n">
+      <c r="D243" s="21" t="n">
         <f aca="false">AND((D184&lt;= D16),(D184 &gt;= 0),(D72&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E243" s="12" t="n">
+      <c r="E243" s="21" t="n">
         <f aca="false">AND((E184&lt;= E16),(E184 &gt;= 0),(E72&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F243" s="12" t="n">
+      <c r="F243" s="21" t="n">
         <f aca="false">AND((F184&lt;= F16),(F184 &gt;= 0),(F72&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6252,23 +6253,23 @@
       <c r="A244" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="B244" s="12" t="n">
+      <c r="B244" s="21" t="n">
         <f aca="false">AND((B185&lt;= B17),(B185 &gt;= 0),(B73&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C244" s="12" t="n">
+      <c r="C244" s="21" t="n">
         <f aca="false">AND((C185&lt;= C17),(C185 &gt;= 0),(C73&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D244" s="12" t="n">
+      <c r="D244" s="21" t="n">
         <f aca="false">AND((D185&lt;= D17),(D185 &gt;= 0),(D73&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E244" s="12" t="n">
+      <c r="E244" s="21" t="n">
         <f aca="false">AND((E185&lt;= E17),(E185 &gt;= 0),(E73&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F244" s="12" t="n">
+      <c r="F244" s="21" t="n">
         <f aca="false">AND((F185&lt;= F17),(F185 &gt;= 0),(F73&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6277,23 +6278,23 @@
       <c r="A245" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="B245" s="12" t="n">
+      <c r="B245" s="21" t="n">
         <f aca="false">AND((B186&lt;= B18),(B186 &gt;= 0),(B74&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C245" s="12" t="n">
+      <c r="C245" s="21" t="n">
         <f aca="false">AND((C186&lt;= C18),(C186 &gt;= 0),(C74&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D245" s="12" t="n">
+      <c r="D245" s="21" t="n">
         <f aca="false">AND((D186&lt;= D18),(D186 &gt;= 0),(D74&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="E245" s="12" t="n">
+      <c r="E245" s="21" t="n">
         <f aca="false">AND((E186&lt;= E18),(E186 &gt;= 0),(E74&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F245" s="12" t="n">
+      <c r="F245" s="21" t="n">
         <f aca="false">AND((F186&lt;= F18),(F186 &gt;= 0),(F74&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6302,23 +6303,23 @@
       <c r="A246" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="B246" s="12" t="n">
+      <c r="B246" s="21" t="n">
         <f aca="false">AND((B187&lt;= B19),(B187 &gt;= 0),(B75&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C246" s="12" t="n">
+      <c r="C246" s="21" t="n">
         <f aca="false">AND((C187&lt;= C19),(C187 &gt;= 0),(C75&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D246" s="12" t="n">
+      <c r="D246" s="21" t="n">
         <f aca="false">AND((D187&lt;= D19),(D187 &gt;= 0),(D75&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E246" s="12" t="n">
+      <c r="E246" s="21" t="n">
         <f aca="false">AND((E187&lt;= E19),(E187 &gt;= 0),(E75&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F246" s="12" t="n">
+      <c r="F246" s="21" t="n">
         <f aca="false">AND((F187&lt;= F19),(F187 &gt;= 0),(F75&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6327,23 +6328,23 @@
       <c r="A247" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="B247" s="12" t="n">
+      <c r="B247" s="21" t="n">
         <f aca="false">AND((B188&lt;= B20),(B188 &gt;= 0),(B76&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C247" s="12" t="n">
+      <c r="C247" s="21" t="n">
         <f aca="false">AND((C188&lt;= C20),(C188 &gt;= 0),(C76&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D247" s="12" t="n">
+      <c r="D247" s="21" t="n">
         <f aca="false">AND((D188&lt;= D20),(D188 &gt;= 0),(D76&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E247" s="12" t="n">
+      <c r="E247" s="21" t="n">
         <f aca="false">AND((E188&lt;= E20),(E188 &gt;= 0),(E76&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F247" s="12" t="n">
+      <c r="F247" s="21" t="n">
         <f aca="false">AND((F188&lt;= F20),(F188 &gt;= 0),(F76&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6352,23 +6353,23 @@
       <c r="A248" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="B248" s="12" t="n">
+      <c r="B248" s="21" t="n">
         <f aca="false">AND((B189&lt;= B21),(B189 &gt;= 0),(B77&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C248" s="12" t="n">
+      <c r="C248" s="21" t="n">
         <f aca="false">AND((C189&lt;= C21),(C189 &gt;= 0),(C77&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D248" s="12" t="n">
+      <c r="D248" s="21" t="n">
         <f aca="false">AND((D189&lt;= D21),(D189 &gt;= 0),(D77&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E248" s="12" t="n">
+      <c r="E248" s="21" t="n">
         <f aca="false">AND((E189&lt;= E21),(E189 &gt;= 0),(E77&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F248" s="12" t="n">
+      <c r="F248" s="21" t="n">
         <f aca="false">AND((F189&lt;= F21),(F189 &gt;= 0),(F77&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6377,23 +6378,23 @@
       <c r="A249" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="B249" s="12" t="n">
+      <c r="B249" s="21" t="n">
         <f aca="false">AND((B190&lt;= B22),(B190 &gt;= 0),(B78&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C249" s="12" t="n">
+      <c r="C249" s="21" t="n">
         <f aca="false">AND((C190&lt;= C22),(C190 &gt;= 0),(C78&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D249" s="12" t="n">
+      <c r="D249" s="21" t="n">
         <f aca="false">AND((D190&lt;= D22),(D190 &gt;= 0),(D78&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E249" s="12" t="n">
+      <c r="E249" s="21" t="n">
         <f aca="false">AND((E190&lt;= E22),(E190 &gt;= 0),(E78&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F249" s="12" t="n">
+      <c r="F249" s="21" t="n">
         <f aca="false">AND((F190&lt;= F22),(F190 &gt;= 0),(F78&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6402,23 +6403,23 @@
       <c r="A250" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="B250" s="12" t="n">
+      <c r="B250" s="21" t="n">
         <f aca="false">AND((B191&lt;= B23),(B191 &gt;= 0),(B79&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C250" s="12" t="n">
+      <c r="C250" s="21" t="n">
         <f aca="false">AND((C191&lt;= C23),(C191 &gt;= 0),(C79&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D250" s="12" t="n">
+      <c r="D250" s="21" t="n">
         <f aca="false">AND((D191&lt;= D23),(D191 &gt;= 0),(D79&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E250" s="12" t="n">
+      <c r="E250" s="21" t="n">
         <f aca="false">AND((E191&lt;= E23),(E191 &gt;= 0),(E79&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F250" s="12" t="n">
+      <c r="F250" s="21" t="n">
         <f aca="false">AND((F191&lt;= F23),(F191 &gt;= 0),(F79&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6427,23 +6428,23 @@
       <c r="A251" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="B251" s="12" t="n">
+      <c r="B251" s="21" t="n">
         <f aca="false">AND((B192&lt;= B24),(B192 &gt;= 0),(B80&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C251" s="12" t="n">
+      <c r="C251" s="21" t="n">
         <f aca="false">AND((C192&lt;= C24),(C192 &gt;= 0),(C80&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="D251" s="12" t="n">
+      <c r="D251" s="21" t="n">
         <f aca="false">AND((D192&lt;= D24),(D192 &gt;= 0),(D80&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E251" s="12" t="n">
+      <c r="E251" s="21" t="n">
         <f aca="false">AND((E192&lt;= E24),(E192 &gt;= 0),(E80&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F251" s="12" t="n">
+      <c r="F251" s="21" t="n">
         <f aca="false">AND((F192&lt;= F24),(F192 &gt;= 0),(F80&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6452,23 +6453,23 @@
       <c r="A252" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="B252" s="12" t="n">
+      <c r="B252" s="21" t="n">
         <f aca="false">AND((B193&lt;= B25),(B193 &gt;= 0),(B81&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C252" s="12" t="n">
+      <c r="C252" s="21" t="n">
         <f aca="false">AND((C193&lt;= C25),(C193 &gt;= 0),(C81&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D252" s="12" t="n">
+      <c r="D252" s="21" t="n">
         <f aca="false">AND((D193&lt;= D25),(D193 &gt;= 0),(D81&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E252" s="12" t="n">
+      <c r="E252" s="21" t="n">
         <f aca="false">AND((E193&lt;= E25),(E193 &gt;= 0),(E81&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F252" s="12" t="n">
+      <c r="F252" s="21" t="n">
         <f aca="false">AND((F193&lt;= F25),(F193 &gt;= 0),(F81&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6477,23 +6478,23 @@
       <c r="A253" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="B253" s="12" t="n">
+      <c r="B253" s="21" t="n">
         <f aca="false">AND((B194&lt;= B26),(B194 &gt;= 0),(B82&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C253" s="12" t="n">
+      <c r="C253" s="21" t="n">
         <f aca="false">AND((C194&lt;= C26),(C194 &gt;= 0),(C82&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D253" s="12" t="n">
+      <c r="D253" s="21" t="n">
         <f aca="false">AND((D194&lt;= D26),(D194 &gt;= 0),(D82&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E253" s="12" t="n">
+      <c r="E253" s="21" t="n">
         <f aca="false">AND((E194&lt;= E26),(E194 &gt;= 0),(E82&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F253" s="12" t="n">
+      <c r="F253" s="21" t="n">
         <f aca="false">AND((F194&lt;= F26),(F194 &gt;= 0),(F82&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6502,23 +6503,23 @@
       <c r="A254" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="B254" s="12" t="n">
+      <c r="B254" s="21" t="n">
         <f aca="false">AND((B195&lt;= B27),(B195 &gt;= 0),(B83&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C254" s="12" t="n">
+      <c r="C254" s="21" t="n">
         <f aca="false">AND((C195&lt;= C27),(C195 &gt;= 0),(C83&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D254" s="12" t="n">
+      <c r="D254" s="21" t="n">
         <f aca="false">AND((D195&lt;= D27),(D195 &gt;= 0),(D83&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E254" s="12" t="n">
+      <c r="E254" s="21" t="n">
         <f aca="false">AND((E195&lt;= E27),(E195 &gt;= 0),(E83&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F254" s="12" t="n">
+      <c r="F254" s="21" t="n">
         <f aca="false">AND((F195&lt;= F27),(F195 &gt;= 0),(F83&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6527,23 +6528,23 @@
       <c r="A255" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="B255" s="12" t="n">
+      <c r="B255" s="21" t="n">
         <f aca="false">AND((B196&lt;= B28),(B196 &gt;= 0),(B84&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C255" s="12" t="n">
+      <c r="C255" s="21" t="n">
         <f aca="false">AND((C196&lt;= C28),(C196 &gt;= 0),(C84&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D255" s="12" t="n">
+      <c r="D255" s="21" t="n">
         <f aca="false">AND((D196&lt;= D28),(D196 &gt;= 0),(D84&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E255" s="12" t="n">
+      <c r="E255" s="21" t="n">
         <f aca="false">AND((E196&lt;= E28),(E196 &gt;= 0),(E84&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F255" s="12" t="n">
+      <c r="F255" s="21" t="n">
         <f aca="false">AND((F196&lt;= F28),(F196 &gt;= 0),(F84&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6552,23 +6553,23 @@
       <c r="A256" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="B256" s="12" t="n">
+      <c r="B256" s="21" t="n">
         <f aca="false">AND((B197&lt;= B29),(B197 &gt;= 0),(B85&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C256" s="12" t="n">
+      <c r="C256" s="21" t="n">
         <f aca="false">AND((C197&lt;= C29),(C197 &gt;= 0),(C85&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D256" s="12" t="n">
+      <c r="D256" s="21" t="n">
         <f aca="false">AND((D197&lt;= D29),(D197 &gt;= 0),(D85&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E256" s="12" t="n">
+      <c r="E256" s="21" t="n">
         <f aca="false">AND((E197&lt;= E29),(E197 &gt;= 0),(E85&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F256" s="12" t="n">
+      <c r="F256" s="21" t="n">
         <f aca="false">AND((F197&lt;= F29),(F197 &gt;= 0),(F85&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6577,23 +6578,23 @@
       <c r="A257" s="10" t="n">
         <v>23</v>
       </c>
-      <c r="B257" s="12" t="n">
+      <c r="B257" s="21" t="n">
         <f aca="false">AND((B198&lt;= B30),(B198 &gt;= 0),(B86&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C257" s="12" t="n">
+      <c r="C257" s="21" t="n">
         <f aca="false">AND((C198&lt;= C30),(C198 &gt;= 0),(C86&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D257" s="12" t="n">
+      <c r="D257" s="21" t="n">
         <f aca="false">AND((D198&lt;= D30),(D198 &gt;= 0),(D86&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E257" s="12" t="n">
+      <c r="E257" s="21" t="n">
         <f aca="false">AND((E198&lt;= E30),(E198 &gt;= 0),(E86&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F257" s="12" t="n">
+      <c r="F257" s="21" t="n">
         <f aca="false">AND((F198&lt;= F30),(F198 &gt;= 0),(F86&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6602,23 +6603,23 @@
       <c r="A258" s="10" t="n">
         <v>24</v>
       </c>
-      <c r="B258" s="12" t="n">
+      <c r="B258" s="21" t="n">
         <f aca="false">AND((B199&lt;= B31),(B199 &gt;= 0),(B87&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C258" s="12" t="n">
+      <c r="C258" s="21" t="n">
         <f aca="false">AND((C199&lt;= C31),(C199 &gt;= 0),(C87&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D258" s="12" t="n">
+      <c r="D258" s="21" t="n">
         <f aca="false">AND((D199&lt;= D31),(D199 &gt;= 0),(D87&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E258" s="12" t="n">
+      <c r="E258" s="21" t="n">
         <f aca="false">AND((E199&lt;= E31),(E199 &gt;= 0),(E87&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F258" s="12" t="n">
+      <c r="F258" s="21" t="n">
         <f aca="false">AND((F199&lt;= F31),(F199 &gt;= 0),(F87&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6627,23 +6628,23 @@
       <c r="A259" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="B259" s="12" t="n">
+      <c r="B259" s="21" t="n">
         <f aca="false">AND((B200&lt;= B32),(B200 &gt;= 0),(B88&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C259" s="12" t="n">
+      <c r="C259" s="21" t="n">
         <f aca="false">AND((C200&lt;= C32),(C200 &gt;= 0),(C88&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D259" s="12" t="n">
+      <c r="D259" s="21" t="n">
         <f aca="false">AND((D200&lt;= D32),(D200 &gt;= 0),(D88&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E259" s="12" t="n">
+      <c r="E259" s="21" t="n">
         <f aca="false">AND((E200&lt;= E32),(E200 &gt;= 0),(E88&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F259" s="12" t="n">
+      <c r="F259" s="21" t="n">
         <f aca="false">AND((F200&lt;= F32),(F200 &gt;= 0),(F88&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6652,23 +6653,23 @@
       <c r="A260" s="10" t="n">
         <v>26</v>
       </c>
-      <c r="B260" s="12" t="n">
+      <c r="B260" s="21" t="n">
         <f aca="false">AND((B201&lt;= B33),(B201 &gt;= 0),(B89&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C260" s="12" t="n">
+      <c r="C260" s="21" t="n">
         <f aca="false">AND((C201&lt;= C33),(C201 &gt;= 0),(C89&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D260" s="12" t="n">
+      <c r="D260" s="21" t="n">
         <f aca="false">AND((D201&lt;= D33),(D201 &gt;= 0),(D89&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E260" s="12" t="n">
+      <c r="E260" s="21" t="n">
         <f aca="false">AND((E201&lt;= E33),(E201 &gt;= 0),(E89&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F260" s="12" t="n">
+      <c r="F260" s="21" t="n">
         <f aca="false">AND((F201&lt;= F33),(F201 &gt;= 0),(F89&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6677,23 +6678,23 @@
       <c r="A261" s="10" t="n">
         <v>27</v>
       </c>
-      <c r="B261" s="12" t="n">
+      <c r="B261" s="21" t="n">
         <f aca="false">AND((B202&lt;= B34),(B202 &gt;= 0),(B90&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C261" s="12" t="n">
+      <c r="C261" s="21" t="n">
         <f aca="false">AND((C202&lt;= C34),(C202 &gt;= 0),(C90&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D261" s="12" t="n">
+      <c r="D261" s="21" t="n">
         <f aca="false">AND((D202&lt;= D34),(D202 &gt;= 0),(D90&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E261" s="12" t="n">
+      <c r="E261" s="21" t="n">
         <f aca="false">AND((E202&lt;= E34),(E202 &gt;= 0),(E90&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F261" s="12" t="n">
+      <c r="F261" s="21" t="n">
         <f aca="false">AND((F202&lt;= F34),(F202 &gt;= 0),(F90&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6702,23 +6703,23 @@
       <c r="A262" s="10" t="n">
         <v>28</v>
       </c>
-      <c r="B262" s="12" t="n">
+      <c r="B262" s="21" t="n">
         <f aca="false">AND((B203&lt;= B35),(B203 &gt;= 0),(B91&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C262" s="12" t="n">
+      <c r="C262" s="21" t="n">
         <f aca="false">AND((C203&lt;= C35),(C203 &gt;= 0),(C91&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D262" s="12" t="n">
+      <c r="D262" s="21" t="n">
         <f aca="false">AND((D203&lt;= D35),(D203 &gt;= 0),(D91&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E262" s="12" t="n">
+      <c r="E262" s="21" t="n">
         <f aca="false">AND((E203&lt;= E35),(E203 &gt;= 0),(E91&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F262" s="12" t="n">
+      <c r="F262" s="21" t="n">
         <f aca="false">AND((F203&lt;= F35),(F203 &gt;= 0),(F91&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6727,23 +6728,23 @@
       <c r="A263" s="10" t="n">
         <v>29</v>
       </c>
-      <c r="B263" s="12" t="n">
+      <c r="B263" s="21" t="n">
         <f aca="false">AND((B204&lt;= B36),(B204 &gt;= 0),(B92&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C263" s="12" t="n">
+      <c r="C263" s="21" t="n">
         <f aca="false">AND((C204&lt;= C36),(C204 &gt;= 0),(C92&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D263" s="12" t="n">
+      <c r="D263" s="21" t="n">
         <f aca="false">AND((D204&lt;= D36),(D204 &gt;= 0),(D92&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E263" s="12" t="n">
+      <c r="E263" s="21" t="n">
         <f aca="false">AND((E204&lt;= E36),(E204 &gt;= 0),(E92&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F263" s="12" t="n">
+      <c r="F263" s="21" t="n">
         <f aca="false">AND((F204&lt;= F36),(F204 &gt;= 0),(F92&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6752,23 +6753,23 @@
       <c r="A264" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="B264" s="12" t="n">
+      <c r="B264" s="21" t="n">
         <f aca="false">AND((B205&lt;= B37),(B205 &gt;= 0),(B93&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C264" s="12" t="n">
+      <c r="C264" s="21" t="n">
         <f aca="false">AND((C205&lt;= C37),(C205 &gt;= 0),(C93&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D264" s="12" t="n">
+      <c r="D264" s="21" t="n">
         <f aca="false">AND((D205&lt;= D37),(D205 &gt;= 0),(D93&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E264" s="12" t="n">
+      <c r="E264" s="21" t="n">
         <f aca="false">AND((E205&lt;= E37),(E205 &gt;= 0),(E93&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F264" s="12" t="n">
+      <c r="F264" s="21" t="n">
         <f aca="false">AND((F205&lt;= F37),(F205 &gt;= 0),(F93&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6777,23 +6778,23 @@
       <c r="A265" s="10" t="n">
         <v>31</v>
       </c>
-      <c r="B265" s="12" t="n">
+      <c r="B265" s="21" t="n">
         <f aca="false">AND((B206&lt;= B38),(B206 &gt;= 0),(B94&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C265" s="12" t="n">
+      <c r="C265" s="21" t="n">
         <f aca="false">AND((C206&lt;= C38),(C206 &gt;= 0),(C94&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D265" s="12" t="n">
+      <c r="D265" s="21" t="n">
         <f aca="false">AND((D206&lt;= D38),(D206 &gt;= 0),(D94&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E265" s="12" t="n">
+      <c r="E265" s="21" t="n">
         <f aca="false">AND((E206&lt;= E38),(E206 &gt;= 0),(E94&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F265" s="12" t="n">
+      <c r="F265" s="21" t="n">
         <f aca="false">AND((F206&lt;= F38),(F206 &gt;= 0),(F94&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6802,23 +6803,23 @@
       <c r="A266" s="10" t="n">
         <v>32</v>
       </c>
-      <c r="B266" s="12" t="n">
+      <c r="B266" s="21" t="n">
         <f aca="false">AND((B207&lt;= B39),(B207 &gt;= 0),(B95&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C266" s="12" t="n">
+      <c r="C266" s="21" t="n">
         <f aca="false">AND((C207&lt;= C39),(C207 &gt;= 0),(C95&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D266" s="12" t="n">
+      <c r="D266" s="21" t="n">
         <f aca="false">AND((D207&lt;= D39),(D207 &gt;= 0),(D95&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E266" s="12" t="n">
+      <c r="E266" s="21" t="n">
         <f aca="false">AND((E207&lt;= E39),(E207 &gt;= 0),(E95&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F266" s="12" t="n">
+      <c r="F266" s="21" t="n">
         <f aca="false">AND((F207&lt;= F39),(F207 &gt;= 0),(F95&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6827,23 +6828,23 @@
       <c r="A267" s="10" t="n">
         <v>33</v>
       </c>
-      <c r="B267" s="12" t="n">
+      <c r="B267" s="21" t="n">
         <f aca="false">AND((B208&lt;= B40),(B208 &gt;= 0),(B96&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C267" s="12" t="n">
+      <c r="C267" s="21" t="n">
         <f aca="false">AND((C208&lt;= C40),(C208 &gt;= 0),(C96&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D267" s="12" t="n">
+      <c r="D267" s="21" t="n">
         <f aca="false">AND((D208&lt;= D40),(D208 &gt;= 0),(D96&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E267" s="12" t="n">
+      <c r="E267" s="21" t="n">
         <f aca="false">AND((E208&lt;= E40),(E208 &gt;= 0),(E96&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F267" s="12" t="n">
+      <c r="F267" s="21" t="n">
         <f aca="false">AND((F208&lt;= F40),(F208 &gt;= 0),(F96&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6852,23 +6853,23 @@
       <c r="A268" s="10" t="n">
         <v>34</v>
       </c>
-      <c r="B268" s="12" t="n">
+      <c r="B268" s="21" t="n">
         <f aca="false">AND((B209&lt;= B41),(B209 &gt;= 0),(B97&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C268" s="12" t="n">
+      <c r="C268" s="21" t="n">
         <f aca="false">AND((C209&lt;= C41),(C209 &gt;= 0),(C97&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D268" s="12" t="n">
+      <c r="D268" s="21" t="n">
         <f aca="false">AND((D209&lt;= D41),(D209 &gt;= 0),(D97&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E268" s="12" t="n">
+      <c r="E268" s="21" t="n">
         <f aca="false">AND((E209&lt;= E41),(E209 &gt;= 0),(E97&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F268" s="12" t="n">
+      <c r="F268" s="21" t="n">
         <f aca="false">AND((F209&lt;= F41),(F209 &gt;= 0),(F97&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6877,23 +6878,23 @@
       <c r="A269" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="B269" s="12" t="n">
+      <c r="B269" s="21" t="n">
         <f aca="false">AND((B210&lt;= B42),(B210 &gt;= 0),(B98&gt;=0))</f>
         <v>1</v>
       </c>
-      <c r="C269" s="12" t="n">
+      <c r="C269" s="21" t="n">
         <f aca="false">AND((C210&lt;= C42),(C210 &gt;= 0),(C98&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D269" s="12" t="n">
+      <c r="D269" s="21" t="n">
         <f aca="false">AND((D210&lt;= D42),(D210 &gt;= 0),(D98&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E269" s="12" t="n">
+      <c r="E269" s="21" t="n">
         <f aca="false">AND((E210&lt;= E42),(E210 &gt;= 0),(E98&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F269" s="12" t="n">
+      <c r="F269" s="21" t="n">
         <f aca="false">AND((F210&lt;= F42),(F210 &gt;= 0),(F98&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6902,23 +6903,23 @@
       <c r="A270" s="10" t="n">
         <v>36</v>
       </c>
-      <c r="B270" s="12" t="n">
+      <c r="B270" s="21" t="n">
         <f aca="false">AND((B211&lt;= B43),(B211 &gt;= 0),(B99&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C270" s="12" t="n">
+      <c r="C270" s="21" t="n">
         <f aca="false">AND((C211&lt;= C43),(C211 &gt;= 0),(C99&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D270" s="12" t="n">
+      <c r="D270" s="21" t="n">
         <f aca="false">AND((D211&lt;= D43),(D211 &gt;= 0),(D99&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E270" s="12" t="n">
+      <c r="E270" s="21" t="n">
         <f aca="false">AND((E211&lt;= E43),(E211 &gt;= 0),(E99&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F270" s="12" t="n">
+      <c r="F270" s="21" t="n">
         <f aca="false">AND((F211&lt;= F43),(F211 &gt;= 0),(F99&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6927,23 +6928,23 @@
       <c r="A271" s="10" t="n">
         <v>37</v>
       </c>
-      <c r="B271" s="12" t="n">
+      <c r="B271" s="21" t="n">
         <f aca="false">AND((B212&lt;= B44),(B212 &gt;= 0),(B100&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C271" s="12" t="n">
+      <c r="C271" s="21" t="n">
         <f aca="false">AND((C212&lt;= C44),(C212 &gt;= 0),(C100&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D271" s="12" t="n">
+      <c r="D271" s="21" t="n">
         <f aca="false">AND((D212&lt;= D44),(D212 &gt;= 0),(D100&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E271" s="12" t="n">
+      <c r="E271" s="21" t="n">
         <f aca="false">AND((E212&lt;= E44),(E212 &gt;= 0),(E100&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F271" s="12" t="n">
+      <c r="F271" s="21" t="n">
         <f aca="false">AND((F212&lt;= F44),(F212 &gt;= 0),(F100&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6952,23 +6953,23 @@
       <c r="A272" s="10" t="n">
         <v>38</v>
       </c>
-      <c r="B272" s="12" t="n">
+      <c r="B272" s="21" t="n">
         <f aca="false">AND((B213&lt;= B45),(B213 &gt;= 0),(B101&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C272" s="12" t="n">
+      <c r="C272" s="21" t="n">
         <f aca="false">AND((C213&lt;= C45),(C213 &gt;= 0),(C101&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D272" s="12" t="n">
+      <c r="D272" s="21" t="n">
         <f aca="false">AND((D213&lt;= D45),(D213 &gt;= 0),(D101&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E272" s="12" t="n">
+      <c r="E272" s="21" t="n">
         <f aca="false">AND((E213&lt;= E45),(E213 &gt;= 0),(E101&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F272" s="12" t="n">
+      <c r="F272" s="21" t="n">
         <f aca="false">AND((F213&lt;= F45),(F213 &gt;= 0),(F101&gt;=0))</f>
         <v>0</v>
       </c>
@@ -6977,23 +6978,23 @@
       <c r="A273" s="10" t="n">
         <v>39</v>
       </c>
-      <c r="B273" s="12" t="n">
+      <c r="B273" s="21" t="n">
         <f aca="false">AND((B214&lt;= B46),(B214 &gt;= 0),(B102&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C273" s="12" t="n">
+      <c r="C273" s="21" t="n">
         <f aca="false">AND((C214&lt;= C46),(C214 &gt;= 0),(C102&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D273" s="12" t="n">
+      <c r="D273" s="21" t="n">
         <f aca="false">AND((D214&lt;= D46),(D214 &gt;= 0),(D102&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E273" s="12" t="n">
+      <c r="E273" s="21" t="n">
         <f aca="false">AND((E214&lt;= E46),(E214 &gt;= 0),(E102&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F273" s="12" t="n">
+      <c r="F273" s="21" t="n">
         <f aca="false">AND((F214&lt;= F46),(F214 &gt;= 0),(F102&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7002,23 +7003,23 @@
       <c r="A274" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="B274" s="12" t="n">
+      <c r="B274" s="21" t="n">
         <f aca="false">AND((B215&lt;= B47),(B215 &gt;= 0),(B103&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C274" s="12" t="n">
+      <c r="C274" s="21" t="n">
         <f aca="false">AND((C215&lt;= C47),(C215 &gt;= 0),(C103&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D274" s="12" t="n">
+      <c r="D274" s="21" t="n">
         <f aca="false">AND((D215&lt;= D47),(D215 &gt;= 0),(D103&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E274" s="12" t="n">
+      <c r="E274" s="21" t="n">
         <f aca="false">AND((E215&lt;= E47),(E215 &gt;= 0),(E103&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F274" s="12" t="n">
+      <c r="F274" s="21" t="n">
         <f aca="false">AND((F215&lt;= F47),(F215 &gt;= 0),(F103&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7027,23 +7028,23 @@
       <c r="A275" s="10" t="n">
         <v>41</v>
       </c>
-      <c r="B275" s="12" t="n">
+      <c r="B275" s="21" t="n">
         <f aca="false">AND((B216&lt;= B48),(B216 &gt;= 0),(B104&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C275" s="12" t="n">
+      <c r="C275" s="21" t="n">
         <f aca="false">AND((C216&lt;= C48),(C216 &gt;= 0),(C104&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D275" s="12" t="n">
+      <c r="D275" s="21" t="n">
         <f aca="false">AND((D216&lt;= D48),(D216 &gt;= 0),(D104&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E275" s="12" t="n">
+      <c r="E275" s="21" t="n">
         <f aca="false">AND((E216&lt;= E48),(E216 &gt;= 0),(E104&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F275" s="12" t="n">
+      <c r="F275" s="21" t="n">
         <f aca="false">AND((F216&lt;= F48),(F216 &gt;= 0),(F104&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7052,23 +7053,23 @@
       <c r="A276" s="10" t="n">
         <v>42</v>
       </c>
-      <c r="B276" s="12" t="n">
+      <c r="B276" s="21" t="n">
         <f aca="false">AND((B217&lt;= B49),(B217 &gt;= 0),(B105&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C276" s="12" t="n">
+      <c r="C276" s="21" t="n">
         <f aca="false">AND((C217&lt;= C49),(C217 &gt;= 0),(C105&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D276" s="12" t="n">
+      <c r="D276" s="21" t="n">
         <f aca="false">AND((D217&lt;= D49),(D217 &gt;= 0),(D105&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E276" s="12" t="n">
+      <c r="E276" s="21" t="n">
         <f aca="false">AND((E217&lt;= E49),(E217 &gt;= 0),(E105&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F276" s="12" t="n">
+      <c r="F276" s="21" t="n">
         <f aca="false">AND((F217&lt;= F49),(F217 &gt;= 0),(F105&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7077,23 +7078,23 @@
       <c r="A277" s="10" t="n">
         <v>43</v>
       </c>
-      <c r="B277" s="12" t="n">
+      <c r="B277" s="21" t="n">
         <f aca="false">AND((B218&lt;= B50),(B218 &gt;= 0),(B106&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C277" s="12" t="n">
+      <c r="C277" s="21" t="n">
         <f aca="false">AND((C218&lt;= C50),(C218 &gt;= 0),(C106&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D277" s="12" t="n">
+      <c r="D277" s="21" t="n">
         <f aca="false">AND((D218&lt;= D50),(D218 &gt;= 0),(D106&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E277" s="12" t="n">
+      <c r="E277" s="21" t="n">
         <f aca="false">AND((E218&lt;= E50),(E218 &gt;= 0),(E106&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F277" s="12" t="n">
+      <c r="F277" s="21" t="n">
         <f aca="false">AND((F218&lt;= F50),(F218 &gt;= 0),(F106&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7102,23 +7103,23 @@
       <c r="A278" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="B278" s="12" t="n">
+      <c r="B278" s="21" t="n">
         <f aca="false">AND((B219&lt;= B51),(B219 &gt;= 0),(B107&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C278" s="12" t="n">
+      <c r="C278" s="21" t="n">
         <f aca="false">AND((C219&lt;= C51),(C219 &gt;= 0),(C107&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D278" s="12" t="n">
+      <c r="D278" s="21" t="n">
         <f aca="false">AND((D219&lt;= D51),(D219 &gt;= 0),(D107&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E278" s="12" t="n">
+      <c r="E278" s="21" t="n">
         <f aca="false">AND((E219&lt;= E51),(E219 &gt;= 0),(E107&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F278" s="12" t="n">
+      <c r="F278" s="21" t="n">
         <f aca="false">AND((F219&lt;= F51),(F219 &gt;= 0),(F107&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7127,23 +7128,23 @@
       <c r="A279" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B279" s="12" t="n">
+      <c r="B279" s="21" t="n">
         <f aca="false">AND((B220&lt;= B52),(B220 &gt;= 0),(B108&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C279" s="12" t="n">
+      <c r="C279" s="21" t="n">
         <f aca="false">AND((C220&lt;= C52),(C220 &gt;= 0),(C108&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D279" s="12" t="n">
+      <c r="D279" s="21" t="n">
         <f aca="false">AND((D220&lt;= D52),(D220 &gt;= 0),(D108&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E279" s="12" t="n">
+      <c r="E279" s="21" t="n">
         <f aca="false">AND((E220&lt;= E52),(E220 &gt;= 0),(E108&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F279" s="12" t="n">
+      <c r="F279" s="21" t="n">
         <f aca="false">AND((F220&lt;= F52),(F220 &gt;= 0),(F108&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7152,23 +7153,23 @@
       <c r="A280" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="B280" s="12" t="n">
+      <c r="B280" s="21" t="n">
         <f aca="false">AND((B221&lt;= B53),(B221 &gt;= 0),(B109&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C280" s="12" t="n">
+      <c r="C280" s="21" t="n">
         <f aca="false">AND((C221&lt;= C53),(C221 &gt;= 0),(C109&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D280" s="12" t="n">
+      <c r="D280" s="21" t="n">
         <f aca="false">AND((D221&lt;= D53),(D221 &gt;= 0),(D109&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E280" s="12" t="n">
+      <c r="E280" s="21" t="n">
         <f aca="false">AND((E221&lt;= E53),(E221 &gt;= 0),(E109&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F280" s="12" t="n">
+      <c r="F280" s="21" t="n">
         <f aca="false">AND((F221&lt;= F53),(F221 &gt;= 0),(F109&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7177,23 +7178,23 @@
       <c r="A281" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B281" s="12" t="n">
+      <c r="B281" s="21" t="n">
         <f aca="false">AND((B222&lt;= B54),(B222 &gt;= 0),(B110&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C281" s="12" t="n">
+      <c r="C281" s="21" t="n">
         <f aca="false">AND((C222&lt;= C54),(C222 &gt;= 0),(C110&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D281" s="12" t="n">
+      <c r="D281" s="21" t="n">
         <f aca="false">AND((D222&lt;= D54),(D222 &gt;= 0),(D110&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E281" s="12" t="n">
+      <c r="E281" s="21" t="n">
         <f aca="false">AND((E222&lt;= E54),(E222 &gt;= 0),(E110&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F281" s="12" t="n">
+      <c r="F281" s="21" t="n">
         <f aca="false">AND((F222&lt;= F54),(F222 &gt;= 0),(F110&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7202,23 +7203,23 @@
       <c r="A282" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="B282" s="12" t="n">
+      <c r="B282" s="21" t="n">
         <f aca="false">AND((B223&lt;= B55),(B223 &gt;= 0),(B111&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C282" s="12" t="n">
+      <c r="C282" s="21" t="n">
         <f aca="false">AND((C223&lt;= C55),(C223 &gt;= 0),(C111&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D282" s="12" t="n">
+      <c r="D282" s="21" t="n">
         <f aca="false">AND((D223&lt;= D55),(D223 &gt;= 0),(D111&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E282" s="12" t="n">
+      <c r="E282" s="21" t="n">
         <f aca="false">AND((E223&lt;= E55),(E223 &gt;= 0),(E111&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F282" s="12" t="n">
+      <c r="F282" s="21" t="n">
         <f aca="false">AND((F223&lt;= F55),(F223 &gt;= 0),(F111&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7227,23 +7228,23 @@
       <c r="A283" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="B283" s="12" t="n">
+      <c r="B283" s="21" t="n">
         <f aca="false">AND((B224&lt;= B56),(B224 &gt;= 0),(B112&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C283" s="12" t="n">
+      <c r="C283" s="21" t="n">
         <f aca="false">AND((C224&lt;= C56),(C224 &gt;= 0),(C112&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D283" s="12" t="n">
+      <c r="D283" s="21" t="n">
         <f aca="false">AND((D224&lt;= D56),(D224 &gt;= 0),(D112&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E283" s="12" t="n">
+      <c r="E283" s="21" t="n">
         <f aca="false">AND((E224&lt;= E56),(E224 &gt;= 0),(E112&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F283" s="12" t="n">
+      <c r="F283" s="21" t="n">
         <f aca="false">AND((F224&lt;= F56),(F224 &gt;= 0),(F112&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7252,23 +7253,23 @@
       <c r="A284" s="10" t="n">
         <v>50</v>
       </c>
-      <c r="B284" s="12" t="n">
+      <c r="B284" s="21" t="n">
         <f aca="false">AND((B225&lt;= B57),(B225 &gt;= 0),(B113&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C284" s="12" t="n">
+      <c r="C284" s="21" t="n">
         <f aca="false">AND((C225&lt;= C57),(C225 &gt;= 0),(C113&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D284" s="12" t="n">
+      <c r="D284" s="21" t="n">
         <f aca="false">AND((D225&lt;= D57),(D225 &gt;= 0),(D113&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E284" s="12" t="n">
+      <c r="E284" s="21" t="n">
         <f aca="false">AND((E225&lt;= E57),(E225 &gt;= 0),(E113&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F284" s="12" t="n">
+      <c r="F284" s="21" t="n">
         <f aca="false">AND((F225&lt;= F57),(F225 &gt;= 0),(F113&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7277,23 +7278,23 @@
       <c r="A285" s="10" t="n">
         <v>51</v>
       </c>
-      <c r="B285" s="12" t="n">
+      <c r="B285" s="21" t="n">
         <f aca="false">AND((B226&lt;= B58),(B226 &gt;= 0),(B114&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C285" s="12" t="n">
+      <c r="C285" s="21" t="n">
         <f aca="false">AND((C226&lt;= C58),(C226 &gt;= 0),(C114&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D285" s="12" t="n">
+      <c r="D285" s="21" t="n">
         <f aca="false">AND((D226&lt;= D58),(D226 &gt;= 0),(D114&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E285" s="12" t="n">
+      <c r="E285" s="21" t="n">
         <f aca="false">AND((E226&lt;= E58),(E226 &gt;= 0),(E114&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F285" s="12" t="n">
+      <c r="F285" s="21" t="n">
         <f aca="false">AND((F226&lt;= F58),(F226 &gt;= 0),(F114&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7302,23 +7303,23 @@
       <c r="A286" s="10" t="n">
         <v>52</v>
       </c>
-      <c r="B286" s="12" t="n">
+      <c r="B286" s="21" t="n">
         <f aca="false">AND((B227&lt;= B59),(B227 &gt;= 0),(B115&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C286" s="12" t="n">
+      <c r="C286" s="21" t="n">
         <f aca="false">AND((C227&lt;= C59),(C227 &gt;= 0),(C115&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D286" s="12" t="n">
+      <c r="D286" s="21" t="n">
         <f aca="false">AND((D227&lt;= D59),(D227 &gt;= 0),(D115&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E286" s="12" t="n">
+      <c r="E286" s="21" t="n">
         <f aca="false">AND((E227&lt;= E59),(E227 &gt;= 0),(E115&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F286" s="12" t="n">
+      <c r="F286" s="21" t="n">
         <f aca="false">AND((F227&lt;= F59),(F227 &gt;= 0),(F115&gt;=0))</f>
         <v>0</v>
       </c>
@@ -7327,30 +7328,30 @@
       <c r="A287" s="19" t="n">
         <v>53</v>
       </c>
-      <c r="B287" s="12" t="n">
+      <c r="B287" s="21" t="n">
         <f aca="false">AND((B228&lt;= B60),(B228 &gt;= 0),(B116&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="C287" s="12" t="n">
+      <c r="C287" s="21" t="n">
         <f aca="false">AND((C228&lt;= C60),(C228 &gt;= 0),(C116&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="D287" s="12" t="n">
+      <c r="D287" s="21" t="n">
         <f aca="false">AND((D228&lt;= D60),(D228 &gt;= 0),(D116&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="E287" s="12" t="n">
+      <c r="E287" s="21" t="n">
         <f aca="false">AND((E228&lt;= E60),(E228 &gt;= 0),(E116&gt;=0))</f>
         <v>0</v>
       </c>
-      <c r="F287" s="12" t="n">
+      <c r="F287" s="21" t="n">
         <f aca="false">AND((F228&lt;= F60),(F228 &gt;= 0),(F116&gt;=0))</f>
         <v>0</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B288" s="20"/>
       <c r="C288" s="20"/>
@@ -7361,7 +7362,7 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B289" s="3" t="s">
         <v>5</v>
@@ -8722,7 +8723,7 @@
     </row>
     <row r="345" customFormat="false" ht="58.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B345" s="15"/>
       <c r="C345" s="15"/>
@@ -8731,14 +8732,14 @@
       <c r="F345" s="15"/>
     </row>
     <row r="347" customFormat="false" ht="61.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A347" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B347" s="21"/>
-      <c r="C347" s="21"/>
-      <c r="D347" s="21"/>
-      <c r="E347" s="21"/>
-      <c r="F347" s="21"/>
+      <c r="A347" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B347" s="22"/>
+      <c r="C347" s="22"/>
+      <c r="D347" s="22"/>
+      <c r="E347" s="22"/>
+      <c r="F347" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>